<commit_message>
A2: mint NFTs on IRISnet, TXs for each minted NFT: E424A5239F1FB5B5DF698111AD8A993F9391B8CC23997281FE65182137218C5D 03FB72A529F5CB9C3FCF7511BBAD9E87E46DA14BEA046B39FF79CD32427BF032 9E5879D98778E8777253AF21809B38CD5A17E1ACD3BD618DBACE389294ECAA8A 4B2ADC13B0FFF9FF5FE2C795D89FE6DF3E49D32423B87F2F4EA216ACE1C0B865 AB38CDFA336E84839D66F021006268F74DEF6FE04388DEFEFB16968282D0039A AC2C856CD9467A77111E999A249BCB07BD377A59A6539CC186E5E38940C2FAC8
nft/token ids: arkNFT001 - arkNFT006
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -109,16 +109,46 @@
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
+    <t xml:space="preserve">E424A5239F1FB5B5DF698111AD8A993F9391B8CC23997281FE65182137218C5D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03FB72A529F5CB9C3FCF7511BBAD9E87E46DA14BEA046B39FF79CD32427BF032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9E5879D98778E8777253AF21809B38CD5A17E1ACD3BD618DBACE389294ECAA8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4B2ADC13B0FFF9FF5FE2C795D89FE6DF3E49D32423B87F2F4EA216ACE1C0B865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB38CDFA336E84839D66F021006268F74DEF6FE04388DEFEFB16968282D0039A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC2C856CD9467A77111E999A249BCB07BD377A59A6539CC186E5E38940C2FAC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkNFT006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChainID</t>
+  </si>
+  <si>
     <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft id you minted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChainID</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on dest chain</t>
@@ -468,10 +498,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -512,10 +542,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -556,10 +586,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -600,10 +630,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -639,25 +669,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -693,25 +723,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -747,25 +777,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -801,25 +831,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -855,25 +885,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -909,25 +939,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -948,7 +978,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1006,25 +1036,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1060,25 +1090,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1115,12 +1145,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1157,12 +1187,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1199,12 +1229,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1241,12 +1271,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1265,10 +1295,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1293,11 +1323,75 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1339,21 +1433,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1396,21 +1490,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1453,21 +1547,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1511,21 +1605,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1566,10 +1660,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1610,10 +1704,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A3: transferred nft id 'arkNFT002' to Stargaze via channel 22, evidence: tx hash: FB2F67ED5BD529835544C46D2C1DCB66FA6EF90954DE8A2D169FB1F67509AEC8 token: arkNFT002 source chain: IRISnet target chain: Stargaze denom id on IRISnet: arkprotocol002 class-id in Stargaze: wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/arkprotocol002
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="48">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB2F67ED5BD529835544C46D2C1DCB66FA6EF90954DE8A2D169FB1F67509AEC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/arkprotocol002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on irisnet</t>
@@ -498,10 +507,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -542,10 +551,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -586,10 +595,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -630,10 +639,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -674,20 +683,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -728,20 +737,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -782,20 +791,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -836,20 +845,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -890,20 +899,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -944,20 +953,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1041,20 +1050,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1095,20 +1104,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1145,12 +1154,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1187,12 +1196,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1229,12 +1238,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1271,12 +1280,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1297,8 +1306,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1411,8 +1420,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1444,10 +1453,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1495,16 +1504,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1552,16 +1561,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1610,16 +1619,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1660,10 +1669,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1704,11 +1713,11 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
A4: transferred nft id 'arkNFT003' to Uptick via channel 17, evidence: tx hash: B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3 token: arkNFT003 source chain: IRISnet: target chain: Uptick denom id on IRISnet: arkprotocol002 denom id on Uptick: ibc/326A6F38C0A4460B7F02AC3D936693254314A5F11720FE12DFE3B31036844B7B
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -157,22 +157,25 @@
     <t xml:space="preserve">elgafar-1</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/326A6F38C0A4460B7F02AC3D936693254314A5F11720FE12DFE3B31036844B7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx hash on dest chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
   </si>
   <si>
     <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -197,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -226,6 +229,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +328,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -507,10 +520,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -551,10 +564,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -595,10 +608,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -639,10 +652,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -683,20 +696,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -737,20 +750,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -791,20 +804,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -845,20 +858,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -899,20 +912,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -953,20 +966,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1050,20 +1063,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1104,20 +1117,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1154,138 +1167,138 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1418,9 +1431,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1459,6 +1472,7 @@
         <v>36</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1477,8 +1491,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1503,17 +1517,17 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1561,16 +1575,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1619,16 +1633,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1669,10 +1683,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1713,11 +1727,11 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
A5: backtransfer from Stargaze to IRISnet via channel 207 (channel 22 on Iris), evidence: tx hash: DD4FED371B1856B105424538DAD0997073A835F9BF6E4F753840849A71A68407 token: arkNFT002 source chain: Stargaze target chain: IRISnet cw721/collection contract: stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz denom id on IRISnet: arkprotocol002
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="52">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD4FED371B1856B105424538DAD0997073A835F9BF6E4F753840849A71A68407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-irishub-1</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on dest chain</t>
@@ -200,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,12 +238,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -331,7 +334,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,10 +523,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -564,10 +567,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -608,10 +611,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -652,10 +655,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -696,20 +699,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -750,20 +753,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -804,20 +807,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -858,20 +861,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -912,20 +915,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -966,20 +969,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1063,20 +1066,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1117,20 +1120,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1167,12 +1170,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1209,12 +1212,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1251,12 +1254,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1293,12 +1296,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1434,7 +1437,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1491,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1548,8 +1551,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1581,10 +1584,10 @@
         <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1633,16 +1636,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1683,10 +1686,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1727,10 +1730,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A6: back transfer from Uptick to IRISnet via channel 3 (channel 17 on Iris), evidence: tx hash: 9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE token: arkNFT003 source chain: Uptick target chain: IRISnet denom id on Uptick: ibc/326A6F38C0A4460B7F02AC3D936693254314A5F11720FE12DFE3B31036844B7B denom id on IRISnet: arkprotocol002 classId on Uptick: nft-transfer/channel-3/arkprotocol002
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="51">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -160,31 +160,28 @@
     <t xml:space="preserve">B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc/326A6F38C0A4460B7F02AC3D936693254314A5F11720FE12DFE3B31036844B7B</t>
-  </si>
-  <si>
     <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
     <t xml:space="preserve">DD4FED371B1856B105424538DAD0997073A835F9BF6E4F753840849A71A68407</t>
   </si>
   <si>
-    <t xml:space="preserve">stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz</t>
-  </si>
-  <si>
     <t xml:space="preserve">gon-irishub-1</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
+    <t xml:space="preserve">9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nft-transfer/channel-3/arkprotocol002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dest chain id</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -699,20 +696,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -753,20 +750,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -807,20 +804,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -861,20 +858,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -915,20 +912,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -969,20 +966,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1066,20 +1063,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1120,62 +1117,62 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1212,12 +1209,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1254,12 +1251,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1296,12 +1293,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1492,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1524,13 +1521,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1551,8 +1548,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1578,16 +1575,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1608,8 +1605,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1636,16 +1633,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix classId on task A4
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -160,6 +160,9 @@
     <t xml:space="preserve">B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3</t>
   </si>
   <si>
+    <t xml:space="preserve">nft-transfer/channel-3/arkprotocol002</t>
+  </si>
+  <si>
     <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
@@ -170,9 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft-transfer/channel-3/arkprotocol002</t>
   </si>
   <si>
     <t xml:space="preserve">dest chain id</t>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1434,7 +1434,66 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1459,32 +1518,31 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1492,7 +1550,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1517,65 +1575,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
+      <c r="A2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
@@ -1584,7 +1585,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1605,8 +1606,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,10 +1634,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
provide both: class id (`dest-port/dest-channel/source-classId`) and collection id (cw721 contract address resp denom id=ibc class)
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="55">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -157,13 +157,28 @@
     <t xml:space="preserve">elgafar-1</t>
   </si>
   <si>
+    <t xml:space="preserve">classId:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contract:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz</t>
+  </si>
+  <si>
     <t xml:space="preserve">B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3</t>
   </si>
   <si>
+    <t xml:space="preserve">ibc/326A6F38C0A4460B7F02AC3D936693254314A5F11720FE12DFE3B31036844B7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">nft-transfer/channel-3/arkprotocol002</t>
   </si>
   <si>
-    <t xml:space="preserve">uptick_7000-2</t>
+    <t xml:space="preserve">collection:</t>
   </si>
   <si>
     <t xml:space="preserve">DD4FED371B1856B105424538DAD0997073A835F9BF6E4F753840849A71A68407</t>
@@ -173,9 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
@@ -206,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -235,6 +247,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -306,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,6 +347,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -520,10 +546,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -564,10 +590,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -608,10 +634,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -652,10 +678,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -696,20 +722,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -750,20 +776,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -804,20 +830,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -858,20 +884,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -912,20 +938,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -966,20 +992,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1063,20 +1089,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1117,20 +1143,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1167,12 +1193,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1209,12 +1235,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1251,12 +1277,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1293,12 +1319,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1431,16 +1457,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
   </cols>
@@ -1472,8 +1498,21 @@
       <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1490,10 +1529,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1518,17 +1557,31 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1547,10 +1600,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1576,7 +1629,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>35</v>
@@ -1585,7 +1638,21 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1604,10 +1671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1634,16 +1701,30 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1684,10 +1765,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1728,10 +1809,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup, provide only cw721 contract and ibc class
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -151,21 +151,12 @@
     <t xml:space="preserve">FB2F67ED5BD529835544C46D2C1DCB66FA6EF90954DE8A2D169FB1F67509AEC8</t>
   </si>
   <si>
-    <t xml:space="preserve">wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/arkprotocol002</t>
+    <t xml:space="preserve">stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz</t>
   </si>
   <si>
     <t xml:space="preserve">elgafar-1</t>
   </si>
   <si>
-    <t xml:space="preserve">classId:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contract:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stars1ff06t96hwd96fa3pq7uxgrxqqt3gv4zda444k0kappcr6tcwyzass8e4jz</t>
-  </si>
-  <si>
     <t xml:space="preserve">B6F94772CAF577B8E108A940ACBBD0CE6469E01EE37F85AAC96F3EF858A0FCE3</t>
   </si>
   <si>
@@ -175,16 +166,7 @@
     <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
-    <t xml:space="preserve">nft-transfer/channel-3/arkprotocol002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collection:</t>
-  </si>
-  <si>
     <t xml:space="preserve">DD4FED371B1856B105424538DAD0997073A835F9BF6E4F753840849A71A68407</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gon-irishub-1</t>
   </si>
   <si>
     <t xml:space="preserve">9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE</t>
@@ -218,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,12 +229,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -324,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,10 +323,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -546,10 +518,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -590,10 +562,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -634,10 +606,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -678,10 +650,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -722,20 +694,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -776,20 +748,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -830,20 +802,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -884,20 +856,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -938,20 +910,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -992,20 +964,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1089,20 +1061,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1143,20 +1115,20 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1193,12 +1165,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1235,12 +1207,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1277,12 +1249,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1319,12 +1291,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1432,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1489,7 +1461,7 @@
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1498,20 +1470,11 @@
       <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1531,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1557,32 +1520,23 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>40</v>
+      <c r="A2" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1600,10 +1554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1629,32 +1583,19 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1673,7 +1614,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1701,31 +1642,22 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1765,10 +1697,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1809,10 +1741,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
evidence A7 - A19
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="96">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -172,10 +172,139 @@
     <t xml:space="preserve">9B3C42A86883079934299D3B7DC80B091F0EAF81742C13EA32449B4DE44B1BCE</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft id</t>
+    <t xml:space="preserve">ibc/1AF44A70DC33932D97B133F80122C96DEC2A6F07E44C0C8A95ED517989B1FA39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/A35AB88B7770A3ABBB21C301892FB04C151DBBF3F744FF3BA7742571AB0DA5CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/DA7264DDF5EE7B16BE80803DF686FFC46788FE0B5280F93F6016AFC6498798E8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/AFD0BC139AFA6D8B0A52322F9E8A96BE894D83C008D88CF99D4BA5ED530210BF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/9A752A6188C0FF328808276E015439BDB0BEEBEB28667EC84A4FCCF5AA617FB8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iris tx nft-transfer transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3CA799F47011E8E3420F09ECF7BE01EFAD49B98CDEFD313E47DEE5A43BBA6395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-irishub-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0B30C39E28840F194A475EEEFAA7229FAA0C170314F86951185578B6630C7F40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFFE2B699F9322CE02A613052AD25BA8FCA0E6B95D30E1C544D5BA8AD1618B1C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9E93E97796867AA4D7F685B17C0DF94A2EE3AA1E52C539DF5F9894848D11C744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53C4D03BFF230A4825800278606540DF613ADB224A017A6119CABF27B1CC9F7B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2646786E1D7803A3F21D4F3D2F9419309264D5E3095C1DE51BF31E4460FF40D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9BEE56A670697CEE29559547C069CF1CA221E0D3DC3C6F605C98F21C932C306C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87A95D73ABBC8998FECDB52920CB9B60AFB42E2FDD2365EA57384FB9B1DB560A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFF15D5101217CF0BA0D75C1FFC46682BA3C898F344FFBC82B847A5D33D1B81C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7942106A0202F97CD877A3B4E7757793DC5488FA0944B0B93062745955825E81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D54EDF29006F6AF2F9A8C004B6E54AF15189A194C4362ED09725DDE6F0179FA8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B42C7B6AA2E1A4C17DD7F64C3F754E1E538210F1AC0A214DD4103E05794E72E7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82283C24C3848948BD3133A6CF28A2156DCD078D513EC63755B9A07E63AE6D5E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">656555ED47C2DC1B60FDD454D5090936A1ADB6E893FAE9DF30AE39FEEAEB32CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5C7D61ED27F85BD532039857E9D73823CE27C9C4EA99AF190DDC54911ADF504B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44F3B562B5006E8F1E7BFB0AA2EC6C23DB38860B3088CB31382DA7D1BBFD06C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3B59B0384875421EA1F451391E530DEBAC899718DFDDE15419349A8310D6876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD93A83E8AD2CA5FA227E35F42AFBF223282683C0968A8D6351EB4CE86B191BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5127B21E419AA66D6DA857FC0F896C0D81D7949B8E196196E9B95EB90F26212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71A6D10BD3EDDD9A33C5BA39C2CFE7949FFE6A880F178B4E41C6C92E4055764C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFB66B8F9E54079030B331BE00703E263D1253F7ED91D2094AAD6D5B62C458E9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06FFD1522BC081F36B2960ADF6CCF102EE04BA120882DAD165D62F59F2A546BB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480239C1107823CE95AA4E0D646131ECC23A8A1C516C38471C504A4F48D121E9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9CA0B8DF49AFD672A79F59BBE1CF293974BB31E32C757D386A08E7B5AD89E6E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DA769B51CBB1816E707D437419A2D51FD81199CE5CD6E0D8B423137DD3E9B243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9148D7920C656B7CB2520E0473C93D1C3598699FA92A491DD6F1384A75BA22FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED28F21640F34F323E406EADB2E26DF0C92AB7F678109FA33CBFD3F7E00E58C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41145169C81B7BD39A41CAC9FB539C492C8FD58D99B7336B42EFEE7B99059716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15D178AEB29D8E6964B07798AB10964053E1480E2E70F8D320D8DCAE81806AE8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9715C8D0FB8D7DBE9A0F7BAEA91D15817EAA499BBAAC9381BEA5D7F43F62A434</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -185,6 +314,18 @@
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain	chain id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AEB85ECFE85E806FDA11458325250FD4271A7438BB31C97A11824B074ECBD23A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B39C561FF0393FB5F7DA8C19738CAF1DD42D0CA9562C474C35749B2DED0E2AB0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9FF47D225BC43F354C54090158E1797A326DD64C2B5890359C4A3F2C5042BD9D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD20E42CC08B92082DD864CA1624279590350044A574D10B0598A931D84BB805</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -413,7 +554,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="A2 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,7 +640,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -518,10 +659,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +684,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A2 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,10 +703,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -587,7 +728,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G24" activeCellId="1" sqref="A2 G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,10 +747,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +772,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -650,10 +791,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -672,10 +813,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="A2 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,20 +835,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -726,10 +881,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A2 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,20 +903,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -780,10 +949,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A2 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -802,20 +971,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -834,10 +1017,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A2 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,20 +1039,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -888,10 +1085,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A2 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,20 +1107,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>74</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -942,10 +1153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A2 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -964,20 +1175,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1264,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A2 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,20 +1286,50 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1093,10 +1348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1115,22 +1370,24 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1150,7 +1407,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A2 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1165,12 +1422,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1192,7 +1449,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A2 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1207,12 +1464,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1491,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1249,12 +1506,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1533,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1291,12 +1548,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1575,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A2 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1432,7 +1689,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,7 +1752,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1557,7 +1814,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1614,8 +1871,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1678,7 +1935,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1722,7 +1979,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A2 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1741,10 +1998,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update A12 and A19
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <sheet name="B2" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="B5" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="B6" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="B7" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -202,10 +203,10 @@
     <t xml:space="preserve">ark026</t>
   </si>
   <si>
-    <t xml:space="preserve">iris tx nft-transfer transfer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ark028</t>
+    <t xml:space="preserve">ibc/5264E6AB7F094942F58C755FAD71F7C5F7DC8F9EA6A58AA16A9BA9694678698D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ark151</t>
   </si>
   <si>
     <t xml:space="preserve">3CA799F47011E8E3420F09ECF7BE01EFAD49B98CDEFD313E47DEE5A43BBA6395</t>
@@ -289,22 +290,22 @@
     <t xml:space="preserve">D9CA0B8DF49AFD672A79F59BBE1CF293974BB31E32C757D386A08E7B5AD89E6E</t>
   </si>
   <si>
-    <t xml:space="preserve">DA769B51CBB1816E707D437419A2D51FD81199CE5CD6E0D8B423137DD3E9B243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9148D7920C656B7CB2520E0473C93D1C3598699FA92A491DD6F1384A75BA22FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ED28F21640F34F323E406EADB2E26DF0C92AB7F678109FA33CBFD3F7E00E58C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41145169C81B7BD39A41CAC9FB539C492C8FD58D99B7336B42EFEE7B99059716</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15D178AEB29D8E6964B07798AB10964053E1480E2E70F8D320D8DCAE81806AE8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9715C8D0FB8D7DBE9A0F7BAEA91D15817EAA499BBAAC9381BEA5D7F43F62A434</t>
+    <t xml:space="preserve">258107172329D10A2879B454820C1B0AB57E8124AFE49799A844A82769D833BB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A15BF46DE2706D09F7951267A986890377CB56857D4409188E857146474001D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">176A6C67BA6D9921028FE9B6C12599E1635C48F9DDFD86449A3E005D388ECD19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17217F017ABD2F25F846B95D7E14DCFE535B9DE1801246B27B3B776E364376A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28DD99AE253AE7DB85820CD66C6628907A94452919258F1BDB97B5BB272A3399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10CF3A5C81FC12B55189500E3506F3039B967625B94C70DB763720574CA7AE79</t>
   </si>
   <si>
     <t xml:space="preserve">6BADE38F087662FB2A3B5FE71114B6220E151C3839C32344EBE58DB23BEC26F2</t>
@@ -1275,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1359,7 +1360,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1563,6 +1564,48 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
add B5, B6, and B7
</commit_message>
<xml_diff>
--- a/taitruong/evidence.xlsx
+++ b/taitruong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="103">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -338,10 +338,22 @@
     <t xml:space="preserve">BD20E42CC08B92082DD864CA1624279590350044A574D10B0598A931D84BB805</t>
   </si>
   <si>
-    <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Internal Transfer TxHash on IRISnet</t>
+    <t xml:space="preserve">A28D4C47D418CCCE69F8CFD1F91B9CB3FDD5AA40D12B390648A0217F1E1C1668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9C5AC0E16C034D1519D2139A7A3A32CD10C7D3E4C4DC17570E6A72A3B2E2C10F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B8D72D04D01CFE297F3E1ED194FA9E40EA6E2FA6D0E757F44E52484F34E29117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1749A47D641A9665DA61FB1C0C877E87046FE4636015264235CD403EE63C09B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A57724760F7669D776EADE6F39164F3F699F8A8A1D5D9B77D626F87BE27F4818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33E160228043C0C6658E9BD18CCD0AE89694AD4B160D4F9EC357561953B9F063</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1288,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -1526,10 +1538,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1552,6 +1564,8 @@
         <v>98</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1568,10 +1582,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1586,14 +1600,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1610,10 +1626,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1628,14 +1644,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>